<commit_message>
renamed getdata3.m to pulldata.m, fixed function calling. Some cosmetic changes to marketgrid.m
</commit_message>
<xml_diff>
--- a/Results/marketgrid.xlsx
+++ b/Results/marketgrid.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="20115" windowHeight="9780" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="20115" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="MDD" sheetId="4" r:id="rId1"/>
@@ -2204,11 +2204,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:hiLowLines/>
-        <c:axId val="75771904"/>
-        <c:axId val="75773440"/>
+        <c:axId val="83697664"/>
+        <c:axId val="83699200"/>
       </c:stockChart>
       <c:catAx>
-        <c:axId val="75771904"/>
+        <c:axId val="83697664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2217,7 +2217,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75773440"/>
+        <c:crossAx val="83699200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2225,7 +2225,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75773440"/>
+        <c:axId val="83699200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="115"/>
@@ -2262,7 +2262,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75771904"/>
+        <c:crossAx val="83697664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2307,7 +2307,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="130" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2318,7 +2318,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9312088" cy="6084794"/>
+    <xdr:ext cx="9297865" cy="6066692"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -2630,7 +2630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T322"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>

</xml_diff>